<commit_message>
Added stuff and blue to pink
</commit_message>
<xml_diff>
--- a/Prodtest.xlsx
+++ b/Prodtest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\MyGIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\MyGIT\AJ_Test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87467A23-AB6C-4448-AFD6-C61C169AC9DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6409741F-BE26-4C99-846E-8FF3FDC0CFA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Class name</t>
   </si>
@@ -73,7 +73,13 @@
     <t>hardware</t>
   </si>
   <si>
-    <t>Blue</t>
+    <t>Desktop</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Pink</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +463,24 @@
         <v>35</v>
       </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>1300</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>